<commit_message>
add validation_function to generate a js file of aftervalidatefct..
</commit_message>
<xml_diff>
--- a/conditions.xlsx
+++ b/conditions.xlsx
@@ -68,9 +68,6 @@
     <t>C14</t>
   </si>
   <si>
-    <t>c15</t>
-  </si>
-  <si>
     <t>C16</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>afterValidatefct_phonenumber</t>
+  </si>
+  <si>
+    <t>C15</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,60 +500,60 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="G2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>